<commit_message>
Melhoramento dos requisitos do projeto e repostas para as perguntas de Socioemocional
</commit_message>
<xml_diff>
--- a/TI-PI-Socio/Backlog-Trabalho_Individual.xlsx
+++ b/TI-PI-Socio/Backlog-Trabalho_Individual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d563610f9c74387/@BANDTEC@/1-Semestre/Trabalho Individual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d563610f9c74387/@BANDTEC@/1-Semestre/BandTec-Trabalho_Individual-CCO-2021-1/TI-PI-Socio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{44ACA212-988D-4911-9EAD-DA817202F191}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1025FE31-5F4F-4DD5-881A-D253950A8C73}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{44ACA212-988D-4911-9EAD-DA817202F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E83B10B-4148-46EF-8E8A-2D352551D485}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E7FD288-6B99-4CF6-8E2B-705FDF632C2E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17655" windowHeight="10920" xr2:uid="{2E7FD288-6B99-4CF6-8E2B-705FDF632C2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t xml:space="preserve">Erik Silva Pacheco|02211013 </t>
   </si>
@@ -54,37 +54,58 @@
     <t>Ordem de execusão</t>
   </si>
   <si>
-    <t>Criação do site para postagens de conteúdo de animes, onde os usuários poderão ver informações de animes com uma guia de temporada. Tudo isso será feito com HTML, CSS e a linguagem JavaScript</t>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>Criação de uma página de Cadastro e Login para os usuários possam se conectar a página e com isso interagir com algumas postagens. Tudo isso será feito com HTML, CSS e a linguagem JavaScript</t>
-  </si>
-  <si>
-    <t>Relacionamento com o Cadastro e Login com o Banco de Dados</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>Ter um Dashboard mostrando os animes mais esperados da temporada de acordo com a votação dos usuários. Será feito com ChartJS</t>
-  </si>
-  <si>
     <t>A interface do site deve ser clara e intuitiva</t>
   </si>
   <si>
-    <t>Ter um espaço para que o usuário possar entrar em contato para relatar algum problema com o site ou até mesmo dar ideias para acrescentar no site</t>
-  </si>
-  <si>
-    <t>Armazenar os dados do cadastro do usuário e enviar para o Banco de Dados em nuvem, hospedo na plataforma Microsoft Azure</t>
-  </si>
-  <si>
     <t>Apresentar uma Dashboard com o resultado das votações</t>
   </si>
   <si>
-    <t>Funcional</t>
+    <t>Criação de uma página para notícias de animes, uma página de guia de temporadas onde cada guia mostrará os animes de acordo com sua temporada. Tudo isso será feito com HTML e CSS;</t>
+  </si>
+  <si>
+    <t>Criação de uma página que recomenda um anime aleatória para o usuário assistir. Tudo isso será feito com HTML, CSS e a linguagem JavaScript</t>
+  </si>
+  <si>
+    <t>Criação de uma página de Cadastro e Login para os usuários possam criar uma conta onde poderão ter acesso ao chat público e onde irão avaliar os animes. Tudo isso será feito com HTML, CSS e a linguagem JavaScript e MySQL</t>
+  </si>
+  <si>
+    <t>Criação de uma página de perfil, a qual irá ter as opções de levar para a página do chat público ou para a página de avaliação</t>
+  </si>
+  <si>
+    <t>Criação da página do chat público, onde os usuários poderão conversar entre si</t>
+  </si>
+  <si>
+    <t>Criação de um banco de dados que conterá os usuários cadastrados, as mensagens do chat público, as notícias, as temporadas, os animes e a avaliação dos animes</t>
+  </si>
+  <si>
+    <t>Essenciais</t>
+  </si>
+  <si>
+    <t>Criação de uma página de rank, a qual irá conter os top 5 animes de cada ano, que será feito através das notas dadas pelos usuários cadastrados;</t>
+  </si>
+  <si>
+    <t>Criação de uma página onde os usuários irão dar uma nota para os animes</t>
+  </si>
+  <si>
+    <t>Ter uma página para que o usuário possar entrar em contato para relatar algum problema com o site ou até mesmo dar ideias para acrescentar no site Tudo isso será feito com HTML, CSS e a linguagem JavaScript</t>
+  </si>
+  <si>
+    <t>Importantes</t>
+  </si>
+  <si>
+    <t>Armazenar os dados do cadastro do usuário e enviar para o Banco de Dados;</t>
+  </si>
+  <si>
+    <t>No login os dados inseridos serão comparados com o que tem no banco de dados para permitir que o usuário acesse sua conta no site</t>
+  </si>
+  <si>
+    <t>A página que gera um anime aleatório deve gerar ao clicar num botão</t>
+  </si>
+  <si>
+    <t>Funcionais</t>
+  </si>
+  <si>
+    <t>As mensagens do chat público deverão ser armazena no banco de dados e mostradas no chat do site</t>
   </si>
 </sst>
 </file>
@@ -106,7 +127,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +146,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -149,11 +176,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,23 +228,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,149 +578,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506EF063-22F4-4E93-9CE2-C49613A80BCD}">
-  <dimension ref="B3:H11"/>
+  <dimension ref="C2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="59.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D4" s="6">
+    <row r="4" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7">
+        <v>5</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="7">
+        <v>5</v>
+      </c>
+      <c r="H5" s="7">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+    </row>
+    <row r="6" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D6" s="12">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="7">
+        <v>8</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D7" s="12">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="12">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="7">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="12">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="7">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="12">
         <v>7</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="6">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="7">
+        <v>21</v>
+      </c>
+      <c r="H10" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="12">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="7">
+        <v>13</v>
+      </c>
+      <c r="H11" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="12">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="8">
+        <v>3</v>
+      </c>
+      <c r="H12" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="12">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="8">
+        <v>8</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" s="12">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8">
+        <v>8</v>
+      </c>
+      <c r="H14" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="D15" s="12">
+        <v>12</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8">
+        <v>13</v>
+      </c>
+      <c r="H15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="D16" s="12">
+        <v>13</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8">
+        <v>13</v>
+      </c>
+      <c r="H16" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="12">
+        <v>14</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="6">
-        <v>3</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="F17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8">
+        <v>21</v>
+      </c>
+      <c r="H17" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="D18" s="12">
+        <v>15</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="8">
+        <v>5</v>
+      </c>
+      <c r="H18" s="8">
         <v>7</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D7" s="6">
-        <v>4</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D8" s="6">
-        <v>5</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D9" s="6">
-        <v>6</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D10" s="6">
-        <v>7</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="6">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Organização das notícias, melhoramento no CSS das páginas e alterações no documento geral
</commit_message>
<xml_diff>
--- a/TI-PI-Socio/Backlog-Trabalho_Individual.xlsx
+++ b/TI-PI-Socio/Backlog-Trabalho_Individual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d563610f9c74387/@BANDTEC@/1-Semestre/BandTec-Trabalho_Individual-CCO-2021-1/TI-PI-Socio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{44ACA212-988D-4911-9EAD-DA817202F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E83B10B-4148-46EF-8E8A-2D352551D485}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="8_{44ACA212-988D-4911-9EAD-DA817202F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31EB9E6F-FA2E-4EE9-917F-1B59FEC4971A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17655" windowHeight="10920" xr2:uid="{2E7FD288-6B99-4CF6-8E2B-705FDF632C2E}"/>
+    <workbookView xWindow="-2325" yWindow="-15750" windowWidth="22875" windowHeight="15045" xr2:uid="{2E7FD288-6B99-4CF6-8E2B-705FDF632C2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506EF063-22F4-4E93-9CE2-C49613A80BCD}">
   <dimension ref="C2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>